<commit_message>
Test asdfñ jsdalkfjsdklafj lksdajfksdaj lksdajfklsdjak ljsdlakfjklsadjf kljsdakljlfsdakfkasdkfñl ksdñlakfñlsdafñlsdakfñl kañlsdakfñlsd
</commit_message>
<xml_diff>
--- a/ACUERDOS/BITACORAS Y EVIDENCIA/PARCIAL_1/Bitacora_semana1.xlsx
+++ b/ACUERDOS/BITACORAS Y EVIDENCIA/PARCIAL_1/Bitacora_semana1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\Desktop\ACUERDOS\BITACORAS\PARCIAL_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utcv\Documents\CUATRI 2015C\MATERIAS\Ingenieria de Software I\MATERIAL DE ENSEÑANZA\Parcial 2\3-1- Introduccion al UML\REPOSITORIO.git\trunk\ACUERDOS\BITACORAS Y EVIDENCIA\PARCIAL_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Grupo:</t>
   </si>
@@ -297,6 +297,9 @@
 *Huellitas A. C., en Córdoba.
 *Consultorio dental “Cobix”, en Córdoba.
 *Consultorio médico particular del Dr. Arturo Neri Barrios, en Sn. Nicolás, Córdoba.</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -660,8 +663,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -691,6 +696,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -763,11 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1350,110 +1353,110 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="2:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="30">
         <v>5</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
@@ -1465,71 +1468,71 @@
       <c r="C13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>2</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="19" spans="3:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="3:8" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D15:H15"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="D10:H10"/>
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1545,7 +1548,7 @@
   <dimension ref="B2:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B3" sqref="B3:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,42 +1564,46 @@
     <col min="9" max="9" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="2:11" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
@@ -1646,7 +1653,7 @@
       <c r="F9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="20" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="16" t="s">
@@ -1828,182 +1835,182 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="39"/>
     </row>
     <row r="4" spans="2:21" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="42"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42" t="s">
+      <c r="C6" s="43"/>
+      <c r="D6" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="K6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="43" t="s">
+      <c r="P6" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="44"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
     </row>
     <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="45" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
     </row>
     <row r="9" spans="2:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="53"/>
-      <c r="U9" s="54"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="56"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="18">
         <v>1</v>
       </c>
@@ -2056,17 +2063,17 @@
     <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:U9"/>
     <mergeCell ref="B2:U4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="P6:U6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:U8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>